<commit_message>
style(hardware): :art: change row height (#10)
</commit_message>
<xml_diff>
--- a/hardware/constellation/Truth Table.xlsx
+++ b/hardware/constellation/Truth Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5ccdfd03dce7e7d/Documents/The University of Auckland/Engineering (Part III)/Repositories/compsys301-pathfinding-robot/hardware/constellation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="660" documentId="8_{07DECEAA-4AC2-4365-B31E-6C3BEDF07812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4CB72E5-CBC5-427A-A49F-ECFCB0B27E9F}"/>
+  <xr:revisionPtr revIDLastSave="662" documentId="8_{07DECEAA-4AC2-4365-B31E-6C3BEDF07812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C9E042A-FAC2-448B-9945-B9646CC02493}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="0" windowWidth="33240" windowHeight="20985" activeTab="1" xr2:uid="{767A1D27-FE25-4BDC-9D57-83EB977FC6BE}"/>
+    <workbookView xWindow="7215" yWindow="7680" windowWidth="20760" windowHeight="13410" xr2:uid="{767A1D27-FE25-4BDC-9D57-83EB977FC6BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -286,14 +286,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -301,34 +300,34 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -337,26 +336,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -416,6 +395,26 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -430,19 +429,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}" name="Table1" displayName="Table1" ref="E1:N129" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}" name="Table1" displayName="Table1" ref="E1:N129" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="E1:N129" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A551AE2E-D2A9-4DFB-B3FD-B9A12BEE0313}" name="Middle (Dead-End)" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{28440364-E8DF-4957-9BC9-CDB1C7A15149}" name="Front Left Sensor (Skew)" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{68005D06-C529-4CE4-BC5C-16F1C4701DF2}" name="Front Right Sensor (Skew)" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{F4B70908-229A-4E3D-B553-A4554669198F}" name="Rear Left Sensor (Skew)" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{C5D545A2-DB60-444C-89E5-72551A831C97}" name="Rear Right (Skew)" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{5BD2794C-ECCD-4C90-BBF0-58C3DEDA83BC}" name="Left (Turn)" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{012500B1-249C-4EFD-A733-8F0C2A6407A6}" name="Right (Turn)" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{A0122365-63D3-4593-8877-9067C2CCDD78}" name="Action" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{78020DB1-20ED-4E82-B68F-806E01B4FC1C}" name="Interpretation" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{4C2BEFD8-22D8-4E39-8B7C-DCFDEBEDA5BA}" name="Remarks" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{A551AE2E-D2A9-4DFB-B3FD-B9A12BEE0313}" name="Middle (Dead-End)" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{28440364-E8DF-4957-9BC9-CDB1C7A15149}" name="Front Left Sensor (Skew)" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{68005D06-C529-4CE4-BC5C-16F1C4701DF2}" name="Front Right Sensor (Skew)" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{F4B70908-229A-4E3D-B553-A4554669198F}" name="Rear Left Sensor (Skew)" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{C5D545A2-DB60-444C-89E5-72551A831C97}" name="Rear Right (Skew)" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{5BD2794C-ECCD-4C90-BBF0-58C3DEDA83BC}" name="Left (Turn)" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{012500B1-249C-4EFD-A733-8F0C2A6407A6}" name="Right (Turn)" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{A0122365-63D3-4593-8877-9067C2CCDD78}" name="Action" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{78020DB1-20ED-4E82-B68F-806E01B4FC1C}" name="Interpretation" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{4C2BEFD8-22D8-4E39-8B7C-DCFDEBEDA5BA}" name="Remarks" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,9 +766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E874EEF7-7DE3-42BC-9FFA-2528880F772D}">
   <dimension ref="E1:O129"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L114" sqref="L114:L125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5047,10 +5046,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:L1048576">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"WHITE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"BLACK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5066,668 +5065,668 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C122C8C-3AF1-42C2-AD73-7242DA3B2F53}">
   <dimension ref="E1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="54.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="54.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1"/>
     </row>
-    <row r="2" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+    <row r="2" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M2"/>
     </row>
-    <row r="3" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+    <row r="3" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M3"/>
     </row>
-    <row r="4" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2" t="s">
+    <row r="4" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M4"/>
     </row>
-    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2" t="s">
+    <row r="5" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M5"/>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="1" t="s">
+    <row r="6" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M6"/>
     </row>
-    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
+    <row r="7" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="M7"/>
     </row>
-    <row r="8" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="s">
+    <row r="8" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="M8"/>
     </row>
-    <row r="9" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
+    <row r="9" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
+    <row r="10" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M10"/>
     </row>
-    <row r="11" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
+    <row r="11" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="H11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M11"/>
     </row>
-    <row r="12" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1" t="s">
+    <row r="12" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M12"/>
     </row>
-    <row r="13" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1" t="s">
+    <row r="13" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M13"/>
     </row>
-    <row r="14" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="s">
+    <row r="14" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="s">
+    <row r="15" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>62</v>
       </c>
       <c r="M15"/>
     </row>
-    <row r="16" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
+    <row r="16" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
+    <row r="17" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
+    <row r="18" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="G18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M18"/>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="s">
+    <row r="19" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M19"/>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="s">
+    <row r="20" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M20"/>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1" t="s">
+    <row r="21" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M21"/>
     </row>
-    <row r="22" spans="5:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
+    <row r="22" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="3" t="s">
         <v>50</v>
       </c>
       <c r="M22"/>
     </row>
-    <row r="23" spans="5:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="E23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="s">
+    <row r="23" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="3" t="s">
         <v>50</v>
       </c>
       <c r="M23"/>
     </row>
-    <row r="24" spans="5:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="E24" s="1" t="s">
+    <row r="24" spans="5:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="F24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" s="2" t="s">
         <v>61</v>
       </c>
       <c r="M24"/>

</xml_diff>

<commit_message>
feat(firmware): :zap: make truth table more tolerant of skew
</commit_message>
<xml_diff>
--- a/hardware/constellation/Truth Table.xlsx
+++ b/hardware/constellation/Truth Table.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5ccdfd03dce7e7d/Documents/The University of Auckland/Engineering (Part III)/Repositories/compsys301-pathfinding-robot/hardware/constellation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="662" documentId="8_{07DECEAA-4AC2-4365-B31E-6C3BEDF07812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C9E042A-FAC2-448B-9945-B9646CC02493}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="8_{07DECEAA-4AC2-4365-B31E-6C3BEDF07812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E294C0A0-0486-44E9-9039-FFAACE75C43A}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="7680" windowWidth="20760" windowHeight="13410" xr2:uid="{767A1D27-FE25-4BDC-9D57-83EB977FC6BE}"/>
+    <workbookView xWindow="255" yWindow="315" windowWidth="33225" windowHeight="21330" xr2:uid="{767A1D27-FE25-4BDC-9D57-83EB977FC6BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Full" sheetId="1" r:id="rId1"/>
-    <sheet name="Reduced" sheetId="3" r:id="rId2"/>
+    <sheet name="Iteration 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Full" sheetId="1" r:id="rId2"/>
+    <sheet name="Reduced" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="65">
   <si>
     <t>BLACK</t>
   </si>
@@ -238,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +260,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +278,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -282,23 +295,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -429,39 +503,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}" name="Table1" displayName="Table1" ref="E1:N129" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7296B58C-F0D9-420F-B9DD-E7F5E05C2CE7}" name="Table14" displayName="Table14" ref="E1:N129" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="E1:N129" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A551AE2E-D2A9-4DFB-B3FD-B9A12BEE0313}" name="Middle (Dead-End)" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{28440364-E8DF-4957-9BC9-CDB1C7A15149}" name="Front Left Sensor (Skew)" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{68005D06-C529-4CE4-BC5C-16F1C4701DF2}" name="Front Right Sensor (Skew)" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{F4B70908-229A-4E3D-B553-A4554669198F}" name="Rear Left Sensor (Skew)" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{C5D545A2-DB60-444C-89E5-72551A831C97}" name="Rear Right (Skew)" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{5BD2794C-ECCD-4C90-BBF0-58C3DEDA83BC}" name="Left (Turn)" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{012500B1-249C-4EFD-A733-8F0C2A6407A6}" name="Right (Turn)" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{A0122365-63D3-4593-8877-9067C2CCDD78}" name="Action" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{78020DB1-20ED-4E82-B68F-806E01B4FC1C}" name="Interpretation" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{4C2BEFD8-22D8-4E39-8B7C-DCFDEBEDA5BA}" name="Remarks" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{021C65B9-67C0-4947-B25A-C385BE8336DC}" name="Middle (Dead-End)" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E516259C-75EB-437D-9697-6FCDF2B4ECEB}" name="Front Left Sensor (Skew)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{100ED7D8-2BC6-4371-92CB-FE09DF3DCAD1}" name="Front Right Sensor (Skew)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{3EEF77C8-970E-4C72-AC88-053867C7677B}" name="Rear Left Sensor (Skew)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{991C1607-0EE1-41E2-8651-19E837E73CC2}" name="Rear Right (Skew)" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{79E77985-F367-4A90-85EC-4417C3DF152B}" name="Left (Turn)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1E841469-7F1B-49D1-B01A-5E990712DF38}" name="Right (Turn)" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{28D3824C-542D-484F-B7D6-84DA05F5EE6A}" name="Action" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{303D5631-0464-4AC9-9468-6C810E9C8681}" name="Interpretation" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{9C6168CB-C575-487A-BD6D-F870EBBCFB7B}" name="Remarks" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3148D4C1-8F5B-4794-A907-5444DBD488BE}" name="Table13" displayName="Table13" ref="E1:L24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}" name="Table1" displayName="Table1" ref="E1:N129" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="E1:N129" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A551AE2E-D2A9-4DFB-B3FD-B9A12BEE0313}" name="Middle (Dead-End)" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{28440364-E8DF-4957-9BC9-CDB1C7A15149}" name="Front Left Sensor (Skew)" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{68005D06-C529-4CE4-BC5C-16F1C4701DF2}" name="Front Right Sensor (Skew)" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{F4B70908-229A-4E3D-B553-A4554669198F}" name="Rear Left Sensor (Skew)" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{C5D545A2-DB60-444C-89E5-72551A831C97}" name="Rear Right (Skew)" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{5BD2794C-ECCD-4C90-BBF0-58C3DEDA83BC}" name="Left (Turn)" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{012500B1-249C-4EFD-A733-8F0C2A6407A6}" name="Right (Turn)" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{A0122365-63D3-4593-8877-9067C2CCDD78}" name="Action" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{78020DB1-20ED-4E82-B68F-806E01B4FC1C}" name="Interpretation" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{4C2BEFD8-22D8-4E39-8B7C-DCFDEBEDA5BA}" name="Remarks" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3148D4C1-8F5B-4794-A907-5444DBD488BE}" name="Table13" displayName="Table13" ref="E1:L24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="E1:L24" xr:uid="{6FD6BE2B-47FE-434E-AFC7-DD3B20F757D5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:L24">
     <sortCondition ref="L1:L24"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{796EA8A7-0D71-4262-988E-9ABE343C8ED0}" name="Middle (Dead-End)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{9AA23787-9A57-4F3E-8073-5D64B6DEADE8}" name="Front Left Sensor (Skew)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{D1CA589D-49E9-4EA3-9F65-798646DCEFA1}" name="Front Right Sensor (Skew)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{2C7BEF49-3065-4FC4-9C75-B9226870B565}" name="Rear Left Sensor (Skew)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{CD60FE40-5608-4B09-BE0A-47BBE4DC541E}" name="Rear Right (Skew)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{8926342A-46C2-4F19-922C-84E405D0ECDF}" name="Left (Turn)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{93043778-2F51-46EE-AFB8-F5F2C3936AC8}" name="Right (Turn)" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{2A42F795-802B-466E-BAF7-CDF54B9FD6B6}" name="Action" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{796EA8A7-0D71-4262-988E-9ABE343C8ED0}" name="Middle (Dead-End)" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{9AA23787-9A57-4F3E-8073-5D64B6DEADE8}" name="Front Left Sensor (Skew)" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{D1CA589D-49E9-4EA3-9F65-798646DCEFA1}" name="Front Right Sensor (Skew)" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{2C7BEF49-3065-4FC4-9C75-B9226870B565}" name="Rear Left Sensor (Skew)" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{CD60FE40-5608-4B09-BE0A-47BBE4DC541E}" name="Rear Right (Skew)" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{8926342A-46C2-4F19-922C-84E405D0ECDF}" name="Left (Turn)" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{93043778-2F51-46EE-AFB8-F5F2C3936AC8}" name="Right (Turn)" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{2A42F795-802B-466E-BAF7-CDF54B9FD6B6}" name="Action" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -763,12 +856,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E874EEF7-7DE3-42BC-9FFA-2528880F772D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89668C2D-480F-44CF-B81C-5FD52E785B73}">
   <dimension ref="E1:O129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L114" sqref="L114:L125"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,8 +1066,8 @@
       <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>62</v>
+      <c r="L6" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>20</v>
@@ -1006,8 +1099,8 @@
       <c r="K7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>62</v>
+      <c r="L7" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>21</v>
@@ -1039,8 +1132,8 @@
       <c r="K8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>62</v>
+      <c r="L8" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>22</v>
@@ -1072,8 +1165,8 @@
       <c r="K9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>62</v>
+      <c r="L9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>18</v>
@@ -1105,8 +1198,8 @@
       <c r="K10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>63</v>
+      <c r="L10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>23</v>
@@ -1138,8 +1231,8 @@
       <c r="K11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>63</v>
+      <c r="L11" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>15</v>
@@ -1171,8 +1264,8 @@
       <c r="K12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>63</v>
+      <c r="L12" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>17</v>
@@ -1204,8 +1297,8 @@
       <c r="K13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>63</v>
+      <c r="L13" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>18</v>
@@ -1369,8 +1462,8 @@
       <c r="K18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>62</v>
+      <c r="L18" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>23</v>
@@ -1402,8 +1495,8 @@
       <c r="K19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>62</v>
+      <c r="L19" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>15</v>
@@ -1435,8 +1528,8 @@
       <c r="K20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>62</v>
+      <c r="L20" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>17</v>
@@ -1468,8 +1561,8 @@
       <c r="K21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>62</v>
+      <c r="L21" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>18</v>
@@ -1897,8 +1990,8 @@
       <c r="K34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>63</v>
+      <c r="L34" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>20</v>
@@ -1930,8 +2023,8 @@
       <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>63</v>
+      <c r="L35" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>15</v>
@@ -1963,8 +2056,8 @@
       <c r="K36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>63</v>
+      <c r="L36" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>17</v>
@@ -1996,8 +2089,8 @@
       <c r="K37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>63</v>
+      <c r="L37" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>18</v>
@@ -5044,12 +5137,11 @@
       <c r="O129"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:L1048576">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WHITE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"BLACK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5062,12 +5154,4311 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E874EEF7-7DE3-42BC-9FFA-2528880F772D}">
+  <dimension ref="E1:O129"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O45"/>
+    </row>
+    <row r="46" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="5:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O62"/>
+    </row>
+    <row r="63" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O63"/>
+    </row>
+    <row r="64" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O68"/>
+    </row>
+    <row r="69" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O69"/>
+    </row>
+    <row r="70" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O70"/>
+    </row>
+    <row r="71" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O71"/>
+    </row>
+    <row r="72" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O72"/>
+    </row>
+    <row r="73" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O73"/>
+    </row>
+    <row r="74" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O74"/>
+    </row>
+    <row r="75" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O75"/>
+    </row>
+    <row r="76" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O76"/>
+    </row>
+    <row r="77" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O77"/>
+    </row>
+    <row r="78" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O78"/>
+    </row>
+    <row r="79" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O79"/>
+    </row>
+    <row r="80" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O80"/>
+    </row>
+    <row r="81" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O81"/>
+    </row>
+    <row r="82" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O85"/>
+    </row>
+    <row r="86" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O86"/>
+    </row>
+    <row r="87" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O87"/>
+    </row>
+    <row r="88" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O88"/>
+    </row>
+    <row r="89" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O89"/>
+    </row>
+    <row r="90" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O90"/>
+    </row>
+    <row r="91" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O91"/>
+    </row>
+    <row r="92" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O92"/>
+    </row>
+    <row r="93" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O93"/>
+    </row>
+    <row r="94" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O94"/>
+    </row>
+    <row r="95" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O95"/>
+    </row>
+    <row r="96" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O96"/>
+    </row>
+    <row r="97" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N97" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O97"/>
+    </row>
+    <row r="98" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N98" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O98"/>
+    </row>
+    <row r="99" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O99"/>
+    </row>
+    <row r="100" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O100"/>
+    </row>
+    <row r="101" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O101"/>
+    </row>
+    <row r="102" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O102"/>
+    </row>
+    <row r="103" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O103"/>
+    </row>
+    <row r="104" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O105"/>
+    </row>
+    <row r="106" spans="5:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="E106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O106"/>
+    </row>
+    <row r="107" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O107"/>
+    </row>
+    <row r="108" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O108"/>
+    </row>
+    <row r="109" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N109" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O109"/>
+    </row>
+    <row r="110" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N110" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O110"/>
+    </row>
+    <row r="111" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O111"/>
+    </row>
+    <row r="112" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O112"/>
+    </row>
+    <row r="113" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N113" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O113"/>
+    </row>
+    <row r="114" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N114" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O114"/>
+    </row>
+    <row r="115" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O115"/>
+    </row>
+    <row r="116" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O116"/>
+    </row>
+    <row r="117" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O117"/>
+    </row>
+    <row r="118" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O118"/>
+    </row>
+    <row r="119" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O119"/>
+    </row>
+    <row r="120" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O120"/>
+    </row>
+    <row r="121" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O121"/>
+    </row>
+    <row r="122" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E122" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O122"/>
+    </row>
+    <row r="123" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O123"/>
+    </row>
+    <row r="124" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O124"/>
+    </row>
+    <row r="125" spans="5:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N125" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O125"/>
+    </row>
+    <row r="126" spans="5:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="E126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N126" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O126"/>
+    </row>
+    <row r="127" spans="5:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="E127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O127"/>
+    </row>
+    <row r="128" spans="5:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="E128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O128"/>
+    </row>
+    <row r="129" spans="5:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="E129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O129"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="E1:L1048576">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+      <formula>"WHITE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+      <formula>"BLACK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C122C8C-3AF1-42C2-AD73-7242DA3B2F53}">
   <dimension ref="E1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,15 +10125,15 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:L1048576">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"WHITE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"BLACK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>